<commit_message>
Number of poles classic Turing
</commit_message>
<xml_diff>
--- a/Results/increasingGamma/Classical/nuOfPoles_increasingGamma_Classic.xlsx
+++ b/Results/increasingGamma/Classical/nuOfPoles_increasingGamma_Classic.xlsx
@@ -113,8 +113,8 @@
   </sheetPr>
   <dimension ref="A2:T32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="293" zoomScaleNormal="293" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="293" zoomScaleNormal="293" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V32" activeCellId="0" sqref="V2:V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>